<commit_message>
tested data tables workflow
</commit_message>
<xml_diff>
--- a/Data/date&name.xlsx
+++ b/Data/date&name.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B6B372-E9FF-48B1-8F37-73C1C49DA8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{99B6B372-E9FF-48B1-8F37-73C1C49DA8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C4B306E-9549-46D9-B600-72AE6DC774C8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4170" yWindow="750" windowWidth="22830" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Order Date</t>
   </si>
@@ -35,6 +35,48 @@
   </si>
   <si>
     <t>Sean O'Donnell</t>
+  </si>
+  <si>
+    <t>Brosina Hoffman</t>
+  </si>
+  <si>
+    <t>Andrew Allen</t>
+  </si>
+  <si>
+    <t>Irene Maddox</t>
+  </si>
+  <si>
+    <t>Harold Pawlan</t>
+  </si>
+  <si>
+    <t>Pete Kriz</t>
+  </si>
+  <si>
+    <t>Alejandro Grove</t>
+  </si>
+  <si>
+    <t>Zuschuss Donatelli</t>
+  </si>
+  <si>
+    <t>Ken Black</t>
+  </si>
+  <si>
+    <t>Sandra Flanagan</t>
+  </si>
+  <si>
+    <t>Emily Burns</t>
+  </si>
+  <si>
+    <t>Eric Hoffmann</t>
+  </si>
+  <si>
+    <t>Tracy Blumstein</t>
+  </si>
+  <si>
+    <t>Matt Abelman</t>
+  </si>
+  <si>
+    <t>Gene Hale</t>
   </si>
 </sst>
 </file>
@@ -360,13 +402,13 @@
       <selection activeCell="D37" sqref="A7:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -374,7 +416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42682</v>
       </c>
@@ -382,7 +424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42682</v>
       </c>
@@ -390,7 +432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42533</v>
       </c>
@@ -398,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42288</v>
       </c>
@@ -406,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42288</v>
       </c>
@@ -414,98 +456,253 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>41799</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>42840</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>42709</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>42330</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>42330</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>41954</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>41772</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>41878</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>41878</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>41878</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>42713</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>42713</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>42932</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>42272</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>42385</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>42385</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>42264</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>43027</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>42712</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>